<commit_message>
Startværdier færdige. Merger med version som ikke er square nu
</commit_message>
<xml_diff>
--- a/examples/Abatement/Data/Othdata_dors_3.xlsx
+++ b/examples/Abatement/Data/Othdata_dors_3.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Y" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="28">
   <si>
     <t>mu/n</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>EH</t>
+  </si>
+  <si>
+    <t>NOX</t>
   </si>
 </sst>
 </file>
@@ -427,8 +430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,10 +616,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -656,6 +659,12 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
       <c r="C3" t="s">
         <v>19</v>
       </c>
@@ -685,6 +694,50 @@
         <v>16</v>
       </c>
       <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9">
         <v>0</v>
       </c>
     </row>
@@ -695,10 +748,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -713,6 +766,11 @@
         <v>19</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>